<commit_message>
update:tran and めめ村 skins
</commit_message>
<xml_diff>
--- a/HatTransData.xlsx
+++ b/HatTransData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeHat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4E9FCD-27C6-4FE3-9E5E-307923B040A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B9576-7173-49FF-9747-28220A205649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hat" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>English</t>
   </si>
@@ -327,10 +327,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ミミッキュ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ひなにい作</t>
     <rPh sb="4" eb="5">
       <t>サク</t>
@@ -473,10 +469,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>音割れレイラー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>音割レイラー</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -512,6 +504,25 @@
     <rPh sb="0" eb="1">
       <t>クビ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>化けの皮</t>
+  </si>
+  <si>
+    <t>レイラー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テイラー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gutierrez</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>toliki</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -840,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A68" sqref="A67:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1125,175 +1136,191 @@
         <v>69</v>
       </c>
       <c r="M40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M41" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="M42" t="s">
         <v>73</v>
-      </c>
-      <c r="M42" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="M43" t="s">
         <v>75</v>
-      </c>
-      <c r="M43" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="M44" t="s">
         <v>77</v>
-      </c>
-      <c r="M44" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M47" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M49" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
+        <v>82</v>
+      </c>
+      <c r="M55" t="s">
         <v>83</v>
-      </c>
-      <c r="M55" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="M57" t="s">
         <v>91</v>
-      </c>
-      <c r="M57" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
+        <v>93</v>
+      </c>
+      <c r="M61" t="s">
         <v>94</v>
-      </c>
-      <c r="M61" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
+        <v>97</v>
+      </c>
+      <c r="M63" t="s">
         <v>98</v>
-      </c>
-      <c r="M63" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
+        <v>99</v>
+      </c>
+      <c r="M64" t="s">
         <v>100</v>
-      </c>
-      <c r="M64" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="M65" t="s">
         <v>102</v>
-      </c>
-      <c r="M65" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M66" t="s">
-        <v>104</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>114</v>
+      </c>
+      <c r="M67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>115</v>
+      </c>
+      <c r="M68" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:Miyachi voicerold and voicevox skins
</commit_message>
<xml_diff>
--- a/HatTransData.xlsx
+++ b/HatTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeHat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B9576-7173-49FF-9747-28220A205649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E1B3BF-C7E8-4247-BA86-A82CA6FBF25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7350" yWindow="3825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hat" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="168">
   <si>
     <t>English</t>
   </si>
@@ -523,6 +523,216 @@
   </si>
   <si>
     <t>toliki</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Miyachi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Akane</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>琴葉茜</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Akari</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>紲星あかり</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Aoi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>琴葉葵</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Armachan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アルマちゃん</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Diachan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ディアちゃん</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>flower</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hau</t>
+  </si>
+  <si>
+    <t>雨晴はう</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>鳴花ヒメ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KANATA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カナタ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kotoe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タンゲコトエ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kou</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>水奈瀬コウ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MANA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Metan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>四国めたん</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mikoto</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>鳴花ミコト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NAKO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ナコ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rei</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>足立レイ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>REKO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レコ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ritsu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>波音リツ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rowen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>式狼縁</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sora</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>桜乃そら</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Taigen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>式大元</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tsukuyomichan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>つくよみちゃん</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tsumugi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>春日部つむぎ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yukari</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>結月ゆかり</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yuzuru</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>伊織弓鶴</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ずんだもん</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Zundamon</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>みやち作</t>
+    <rPh sb="3" eb="4">
+      <t>サク</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -851,16 +1061,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q68"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A67:A68"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.625" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="12" width="3.75" customWidth="1"/>
     <col min="13" max="13" width="38.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1323,6 +1533,222 @@
         <v>113</v>
       </c>
     </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>116</v>
+      </c>
+      <c r="M70" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>117</v>
+      </c>
+      <c r="M71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>119</v>
+      </c>
+      <c r="M72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>121</v>
+      </c>
+      <c r="M73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>123</v>
+      </c>
+      <c r="M74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>125</v>
+      </c>
+      <c r="M75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>127</v>
+      </c>
+      <c r="M76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>128</v>
+      </c>
+      <c r="M77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>130</v>
+      </c>
+      <c r="M78" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>132</v>
+      </c>
+      <c r="M79" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>134</v>
+      </c>
+      <c r="M80" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>136</v>
+      </c>
+      <c r="M81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="M82" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>139</v>
+      </c>
+      <c r="M83" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>141</v>
+      </c>
+      <c r="M84" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>143</v>
+      </c>
+      <c r="M85" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="M86" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+      <c r="M87" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>149</v>
+      </c>
+      <c r="M88" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>151</v>
+      </c>
+      <c r="M89" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>153</v>
+      </c>
+      <c r="M90" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="M91" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>157</v>
+      </c>
+      <c r="M92" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>159</v>
+      </c>
+      <c r="M93" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>161</v>
+      </c>
+      <c r="M94" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>163</v>
+      </c>
+      <c r="M95" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>166</v>
+      </c>
+      <c r="M96" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat:new nekowasa hat skin
</commit_message>
<xml_diff>
--- a/HatTransData.xlsx
+++ b/HatTransData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeHat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE20A27-E4C8-4A75-BC08-224FCA089121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952BD975-80E2-4BB8-AFF7-A74450D9D562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="336">
   <si>
     <t>English</t>
   </si>
@@ -1409,6 +1409,14 @@
   </si>
   <si>
     <t>チキン1つ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KindGang</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gチキくーださい</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1739,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="M159" sqref="M159"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1989,6 +1997,14 @@
         <v>295</v>
       </c>
     </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>334</v>
+      </c>
+      <c r="M26" t="s">
+        <v>335</v>
+      </c>
+    </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
     </row>

</xml_diff>

<commit_message>
feat:new hat and fix:hats
</commit_message>
<xml_diff>
--- a/HatTransData.xlsx
+++ b/HatTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeHat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C51064-B82A-4A7A-AE33-BD608552BE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB853196-E8BA-4C53-9652-5505ED822252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hat" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="494">
   <si>
     <t>English</t>
   </si>
@@ -1907,6 +1907,134 @@
   </si>
   <si>
     <t>アイス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AkaneSy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>琴葉茜(Synthesizer V)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AkariAI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AkariTu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>紲星あかり 蕾</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>紲星あかり AI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AoiSy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Chifuyu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>花隈千冬</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Karin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>夏色花梨</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kiritan2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>東北きりたん 私服</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kiritanpo2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>琴葉葵(Synthesizer V)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>東北きりたん 私服(きりたんぽ)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kou2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>水奈瀬コウ(上着あり)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ohoshi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お星</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rikka</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小春六花</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SasaraAI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さとうささら AI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tobari</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>夜語トバリ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TsudumiAI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>すずきつづみ AI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YukariAI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>結月ゆかり AI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yukarisizuku</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>結月ゆかり 雫</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2284,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q258"/>
+  <dimension ref="A1:Q272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="B197" sqref="B197"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138:M272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3190,916 +3318,841 @@
         <v>285</v>
       </c>
     </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>462</v>
+      </c>
+      <c r="M121" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>464</v>
+      </c>
+      <c r="M122" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>465</v>
+      </c>
+      <c r="M123" t="s">
+        <v>466</v>
+      </c>
+    </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
-        <v>168</v>
+        <v>468</v>
       </c>
       <c r="M124" t="s">
-        <v>239</v>
+        <v>476</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
-        <v>169</v>
+        <v>469</v>
       </c>
       <c r="M125" t="s">
-        <v>170</v>
+        <v>470</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>172</v>
+        <v>471</v>
       </c>
       <c r="M126" t="s">
-        <v>171</v>
+        <v>472</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
-        <v>174</v>
+        <v>473</v>
       </c>
       <c r="M127" t="s">
-        <v>173</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>475</v>
       </c>
       <c r="M128" t="s">
-        <v>176</v>
+        <v>477</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>177</v>
+        <v>478</v>
       </c>
       <c r="M129" t="s">
-        <v>178</v>
+        <v>479</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>480</v>
       </c>
       <c r="M130" t="s">
-        <v>180</v>
+        <v>481</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
-        <v>181</v>
+        <v>482</v>
       </c>
       <c r="M131" t="s">
-        <v>182</v>
+        <v>483</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>184</v>
+        <v>484</v>
       </c>
       <c r="M132" t="s">
-        <v>183</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
-        <v>185</v>
+        <v>486</v>
       </c>
       <c r="M133" t="s">
-        <v>186</v>
+        <v>487</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
-        <v>187</v>
+        <v>488</v>
       </c>
       <c r="M134" t="s">
-        <v>188</v>
+        <v>489</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
-        <v>189</v>
+        <v>490</v>
       </c>
       <c r="M135" t="s">
-        <v>190</v>
+        <v>491</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
-        <v>191</v>
+        <v>492</v>
       </c>
       <c r="M136" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A137" t="s">
-        <v>193</v>
-      </c>
-      <c r="M137" t="s">
-        <v>194</v>
+        <v>493</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="M138" t="s">
-        <v>196</v>
+        <v>239</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="M139" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="M140" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="M141" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="M142" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="M143" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="M144" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="M145" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="M146" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="M147" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="M148" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="M149" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="M150" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="M151" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="M152" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="M153" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="M154" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="M155" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="M156" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="M157" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="M158" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="M159" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
-        <v>318</v>
+        <v>211</v>
       </c>
       <c r="M160" t="s">
-        <v>327</v>
+        <v>212</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
-        <v>319</v>
+        <v>213</v>
       </c>
       <c r="M161" t="s">
-        <v>326</v>
+        <v>214</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
-        <v>320</v>
+        <v>215</v>
       </c>
       <c r="M162" t="s">
-        <v>328</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
-        <v>321</v>
+        <v>217</v>
       </c>
       <c r="M163" t="s">
-        <v>329</v>
+        <v>218</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
-        <v>322</v>
+        <v>219</v>
       </c>
       <c r="M164" t="s">
-        <v>330</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
-        <v>323</v>
+        <v>221</v>
       </c>
       <c r="M165" t="s">
-        <v>331</v>
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
-        <v>324</v>
+        <v>223</v>
       </c>
       <c r="M166" t="s">
-        <v>332</v>
+        <v>224</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
-        <v>325</v>
+        <v>225</v>
       </c>
       <c r="M167" t="s">
-        <v>333</v>
+        <v>226</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
-        <v>410</v>
+        <v>227</v>
       </c>
       <c r="M168" t="s">
-        <v>407</v>
+        <v>228</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
-        <v>411</v>
+        <v>229</v>
       </c>
       <c r="M169" t="s">
-        <v>408</v>
+        <v>230</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
-        <v>412</v>
+        <v>234</v>
       </c>
       <c r="M170" t="s">
-        <v>409</v>
+        <v>233</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
-        <v>448</v>
+        <v>231</v>
       </c>
       <c r="M171" t="s">
-        <v>451</v>
+        <v>232</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
-        <v>449</v>
+        <v>235</v>
       </c>
       <c r="M172" t="s">
-        <v>452</v>
+        <v>236</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A173" t="s">
-        <v>450</v>
+        <v>237</v>
       </c>
       <c r="M173" t="s">
-        <v>453</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A174" t="s">
+        <v>318</v>
+      </c>
+      <c r="M174" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>319</v>
+      </c>
+      <c r="M175" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A176" t="s">
+        <v>320</v>
+      </c>
+      <c r="M176" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
+        <v>321</v>
+      </c>
+      <c r="M177" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>322</v>
+      </c>
+      <c r="M178" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
-        <v>286</v>
+        <v>323</v>
       </c>
       <c r="M179" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="M180" t="s">
-        <v>288</v>
+        <v>332</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="M181" t="s">
-        <v>291</v>
+        <v>333</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
-        <v>293</v>
+        <v>410</v>
       </c>
       <c r="M182" t="s">
-        <v>292</v>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
+        <v>411</v>
+      </c>
+      <c r="M183" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A184" t="s">
-        <v>296</v>
+        <v>412</v>
       </c>
       <c r="M184" t="s">
-        <v>297</v>
+        <v>409</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A185" t="s">
-        <v>298</v>
+        <v>448</v>
       </c>
       <c r="M185" t="s">
-        <v>299</v>
+        <v>451</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A186" t="s">
-        <v>310</v>
+        <v>449</v>
       </c>
       <c r="M186" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A189" t="s">
-        <v>302</v>
-      </c>
-      <c r="M189" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A190" t="s">
-        <v>301</v>
-      </c>
-      <c r="B190" t="s">
-        <v>301</v>
-      </c>
-      <c r="M190" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A191" t="s">
-        <v>312</v>
-      </c>
-      <c r="B191" t="s">
-        <v>313</v>
-      </c>
-      <c r="M191" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A192" t="s">
-        <v>343</v>
-      </c>
-      <c r="M192" t="s">
-        <v>342</v>
+        <v>452</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
+        <v>450</v>
+      </c>
+      <c r="M187" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A193" t="s">
-        <v>346</v>
-      </c>
-      <c r="B193" t="s">
-        <v>345</v>
+        <v>286</v>
       </c>
       <c r="M193" t="s">
-        <v>344</v>
+        <v>287</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A194" t="s">
-        <v>456</v>
+        <v>289</v>
       </c>
       <c r="M194" t="s">
-        <v>457</v>
+        <v>288</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A195" t="s">
-        <v>454</v>
+        <v>290</v>
       </c>
       <c r="M195" t="s">
-        <v>455</v>
+        <v>291</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A196" t="s">
-        <v>458</v>
+        <v>293</v>
       </c>
       <c r="M196" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A197" t="s">
-        <v>460</v>
-      </c>
-      <c r="M197" t="s">
-        <v>461</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
+        <v>296</v>
+      </c>
+      <c r="M198" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A199" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="M199" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A200" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="M200" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A201" t="s">
-        <v>309</v>
-      </c>
-      <c r="M201" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A202" t="s">
-        <v>315</v>
-      </c>
-      <c r="B202" t="s">
-        <v>317</v>
-      </c>
-      <c r="M202" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A203" t="s">
-        <v>401</v>
+        <v>302</v>
       </c>
       <c r="M203" t="s">
-        <v>403</v>
+        <v>303</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A204" t="s">
-        <v>402</v>
+        <v>301</v>
+      </c>
+      <c r="B204" t="s">
+        <v>301</v>
       </c>
       <c r="M204" t="s">
-        <v>404</v>
+        <v>300</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A205" t="s">
-        <v>405</v>
+        <v>312</v>
       </c>
       <c r="B205" t="s">
-        <v>405</v>
+        <v>313</v>
       </c>
       <c r="M205" t="s">
-        <v>406</v>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A206" t="s">
+        <v>343</v>
+      </c>
+      <c r="M206" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A207" t="s">
-        <v>347</v>
+        <v>346</v>
+      </c>
+      <c r="B207" t="s">
+        <v>345</v>
       </c>
       <c r="M207" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A208" t="s">
-        <v>349</v>
+        <v>456</v>
       </c>
       <c r="M208" t="s">
-        <v>350</v>
+        <v>457</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A209" t="s">
-        <v>351</v>
+        <v>454</v>
       </c>
       <c r="M209" t="s">
-        <v>352</v>
+        <v>455</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A210" t="s">
-        <v>354</v>
+        <v>458</v>
       </c>
       <c r="M210" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A212" t="s">
-        <v>338</v>
-      </c>
-      <c r="M212" t="s">
-        <v>339</v>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A211" t="s">
+        <v>460</v>
+      </c>
+      <c r="M211" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A213" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
       <c r="M213" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A214" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
-      <c r="D214" s="2"/>
-      <c r="E214" s="2"/>
-      <c r="F214" s="2"/>
-      <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="2"/>
-      <c r="J214" s="2"/>
-      <c r="K214" s="2"/>
-      <c r="L214" s="2"/>
-      <c r="M214" s="2" t="s">
-        <v>356</v>
+      <c r="A214" t="s">
+        <v>305</v>
+      </c>
+      <c r="M214" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A215" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-      <c r="D215" s="2"/>
-      <c r="E215" s="2"/>
-      <c r="F215" s="2"/>
-      <c r="G215" s="2"/>
-      <c r="H215" s="2"/>
-      <c r="I215" s="2"/>
-      <c r="J215" s="2"/>
-      <c r="K215" s="2"/>
-      <c r="L215" s="2"/>
-      <c r="M215" s="2" t="s">
-        <v>358</v>
+      <c r="A215" t="s">
+        <v>309</v>
+      </c>
+      <c r="M215" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A216" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
-      <c r="D216" s="2"/>
-      <c r="E216" s="2"/>
-      <c r="F216" s="2"/>
-      <c r="G216" s="2"/>
-      <c r="H216" s="2"/>
-      <c r="I216" s="2"/>
-      <c r="J216" s="2"/>
-      <c r="K216" s="2"/>
-      <c r="L216" s="2"/>
-      <c r="M216" s="2" t="s">
-        <v>360</v>
+      <c r="A216" t="s">
+        <v>315</v>
+      </c>
+      <c r="B216" t="s">
+        <v>317</v>
+      </c>
+      <c r="M216" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A217" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
-      <c r="D217" s="2"/>
-      <c r="E217" s="2"/>
-      <c r="F217" s="2"/>
-      <c r="G217" s="2"/>
-      <c r="H217" s="2"/>
-      <c r="I217" s="2"/>
-      <c r="J217" s="2"/>
-      <c r="K217" s="2"/>
-      <c r="L217" s="2"/>
-      <c r="M217" s="2" t="s">
-        <v>362</v>
+      <c r="A217" t="s">
+        <v>401</v>
+      </c>
+      <c r="M217" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A218" t="s">
-        <v>446</v>
+        <v>402</v>
       </c>
       <c r="M218" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A220" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
-      <c r="D220" s="2"/>
-      <c r="E220" s="2"/>
-      <c r="F220" s="2"/>
-      <c r="G220" s="2"/>
-      <c r="H220" s="2"/>
-      <c r="I220" s="2"/>
-      <c r="J220" s="2"/>
-      <c r="K220" s="2"/>
-      <c r="L220" s="2"/>
-      <c r="M220" s="2" t="s">
-        <v>364</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
+        <v>405</v>
+      </c>
+      <c r="B219" t="s">
+        <v>405</v>
+      </c>
+      <c r="M219" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A221" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
-      <c r="D221" s="2"/>
-      <c r="E221" s="2"/>
-      <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
-      <c r="H221" s="2"/>
-      <c r="I221" s="2"/>
-      <c r="J221" s="2"/>
-      <c r="K221" s="2"/>
-      <c r="L221" s="2"/>
-      <c r="M221" s="2" t="s">
-        <v>366</v>
+      <c r="A221" t="s">
+        <v>347</v>
+      </c>
+      <c r="M221" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A222" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
-      <c r="D222" s="2"/>
-      <c r="E222" s="2"/>
-      <c r="F222" s="2"/>
-      <c r="G222" s="2"/>
-      <c r="H222" s="2"/>
-      <c r="I222" s="2"/>
-      <c r="J222" s="2"/>
-      <c r="K222" s="2"/>
-      <c r="L222" s="2"/>
-      <c r="M222" s="2" t="s">
-        <v>368</v>
+      <c r="A222" t="s">
+        <v>349</v>
+      </c>
+      <c r="M222" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A223" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
-      <c r="D223" s="2"/>
-      <c r="E223" s="2"/>
-      <c r="F223" s="2"/>
-      <c r="G223" s="2"/>
-      <c r="H223" s="2"/>
-      <c r="I223" s="2"/>
-      <c r="J223" s="2"/>
-      <c r="K223" s="2"/>
-      <c r="L223" s="2"/>
-      <c r="M223" s="2" t="s">
-        <v>370</v>
+      <c r="A223" t="s">
+        <v>351</v>
+      </c>
+      <c r="M223" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A224" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
-      <c r="D224" s="2"/>
-      <c r="E224" s="2"/>
-      <c r="F224" s="2"/>
-      <c r="G224" s="2"/>
-      <c r="H224" s="2"/>
-      <c r="I224" s="2"/>
-      <c r="J224" s="2"/>
-      <c r="K224" s="2"/>
-      <c r="L224" s="2"/>
-      <c r="M224" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A225" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
-      <c r="D225" s="2"/>
-      <c r="E225" s="2"/>
-      <c r="F225" s="2"/>
-      <c r="G225" s="2"/>
-      <c r="H225" s="2"/>
-      <c r="I225" s="2"/>
-      <c r="J225" s="2"/>
-      <c r="K225" s="2"/>
-      <c r="L225" s="2"/>
-      <c r="M225" s="2" t="s">
-        <v>374</v>
+      <c r="A224" t="s">
+        <v>354</v>
+      </c>
+      <c r="M224" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A226" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
-      <c r="D226" s="2"/>
-      <c r="E226" s="2"/>
-      <c r="F226" s="2"/>
-      <c r="G226" s="2"/>
-      <c r="H226" s="2"/>
-      <c r="I226" s="2"/>
-      <c r="J226" s="2"/>
-      <c r="K226" s="2"/>
-      <c r="L226" s="2"/>
-      <c r="M226" s="3" t="s">
-        <v>376</v>
+      <c r="A226" t="s">
+        <v>338</v>
+      </c>
+      <c r="M226" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A227" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
-      <c r="D227" s="2"/>
-      <c r="E227" s="2"/>
-      <c r="F227" s="2"/>
-      <c r="G227" s="2"/>
-      <c r="H227" s="2"/>
-      <c r="I227" s="2"/>
-      <c r="J227" s="2"/>
-      <c r="K227" s="2"/>
-      <c r="L227" s="2"/>
-      <c r="M227" s="3" t="s">
-        <v>378</v>
+      <c r="A227" t="s">
+        <v>340</v>
+      </c>
+      <c r="M227" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A228" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="M228" s="5" t="s">
-        <v>380</v>
+      <c r="A228" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B228" s="2"/>
+      <c r="C228" s="2"/>
+      <c r="D228" s="2"/>
+      <c r="E228" s="2"/>
+      <c r="F228" s="2"/>
+      <c r="G228" s="2"/>
+      <c r="H228" s="2"/>
+      <c r="I228" s="2"/>
+      <c r="J228" s="2"/>
+      <c r="K228" s="2"/>
+      <c r="L228" s="2"/>
+      <c r="M228" s="2" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A229" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="M229" s="6" t="s">
-        <v>382</v>
+      <c r="A229" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="2"/>
+      <c r="M229" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A230" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="M230" s="7" t="s">
-        <v>384</v>
+      <c r="A230" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B230" s="2"/>
+      <c r="C230" s="2"/>
+      <c r="D230" s="2"/>
+      <c r="E230" s="2"/>
+      <c r="F230" s="2"/>
+      <c r="G230" s="2"/>
+      <c r="H230" s="2"/>
+      <c r="I230" s="2"/>
+      <c r="J230" s="2"/>
+      <c r="K230" s="2"/>
+      <c r="L230" s="2"/>
+      <c r="M230" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="231" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A231" s="6" t="s">
-        <v>385</v>
+      <c r="A231" s="2" t="s">
+        <v>361</v>
       </c>
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
@@ -4112,199 +4165,402 @@
       <c r="J231" s="2"/>
       <c r="K231" s="2"/>
       <c r="L231" s="2"/>
-      <c r="M231" s="6" t="s">
+      <c r="M231" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
+        <v>446</v>
+      </c>
+      <c r="M232" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A234" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B234" s="2"/>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
+      <c r="E234" s="2"/>
+      <c r="F234" s="2"/>
+      <c r="G234" s="2"/>
+      <c r="H234" s="2"/>
+      <c r="I234" s="2"/>
+      <c r="J234" s="2"/>
+      <c r="K234" s="2"/>
+      <c r="L234" s="2"/>
+      <c r="M234" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A235" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B235" s="2"/>
+      <c r="C235" s="2"/>
+      <c r="D235" s="2"/>
+      <c r="E235" s="2"/>
+      <c r="F235" s="2"/>
+      <c r="G235" s="2"/>
+      <c r="H235" s="2"/>
+      <c r="I235" s="2"/>
+      <c r="J235" s="2"/>
+      <c r="K235" s="2"/>
+      <c r="L235" s="2"/>
+      <c r="M235" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A236" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B236" s="2"/>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
+      <c r="E236" s="2"/>
+      <c r="F236" s="2"/>
+      <c r="G236" s="2"/>
+      <c r="H236" s="2"/>
+      <c r="I236" s="2"/>
+      <c r="J236" s="2"/>
+      <c r="K236" s="2"/>
+      <c r="L236" s="2"/>
+      <c r="M236" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A237" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B237" s="2"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+      <c r="E237" s="2"/>
+      <c r="F237" s="2"/>
+      <c r="G237" s="2"/>
+      <c r="H237" s="2"/>
+      <c r="I237" s="2"/>
+      <c r="J237" s="2"/>
+      <c r="K237" s="2"/>
+      <c r="L237" s="2"/>
+      <c r="M237" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A238" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B238" s="2"/>
+      <c r="C238" s="2"/>
+      <c r="D238" s="2"/>
+      <c r="E238" s="2"/>
+      <c r="F238" s="2"/>
+      <c r="G238" s="2"/>
+      <c r="H238" s="2"/>
+      <c r="I238" s="2"/>
+      <c r="J238" s="2"/>
+      <c r="K238" s="2"/>
+      <c r="L238" s="2"/>
+      <c r="M238" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A239" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B239" s="2"/>
+      <c r="C239" s="2"/>
+      <c r="D239" s="2"/>
+      <c r="E239" s="2"/>
+      <c r="F239" s="2"/>
+      <c r="G239" s="2"/>
+      <c r="H239" s="2"/>
+      <c r="I239" s="2"/>
+      <c r="J239" s="2"/>
+      <c r="K239" s="2"/>
+      <c r="L239" s="2"/>
+      <c r="M239" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A240" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B240" s="2"/>
+      <c r="C240" s="2"/>
+      <c r="D240" s="2"/>
+      <c r="E240" s="2"/>
+      <c r="F240" s="2"/>
+      <c r="G240" s="2"/>
+      <c r="H240" s="2"/>
+      <c r="I240" s="2"/>
+      <c r="J240" s="2"/>
+      <c r="K240" s="2"/>
+      <c r="L240" s="2"/>
+      <c r="M240" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A241" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B241" s="2"/>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="2"/>
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="2"/>
+      <c r="M241" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A242" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="M242" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A243" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="M243" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A244" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="M244" s="7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A245" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B245" s="2"/>
+      <c r="C245" s="2"/>
+      <c r="D245" s="2"/>
+      <c r="E245" s="2"/>
+      <c r="F245" s="2"/>
+      <c r="G245" s="2"/>
+      <c r="H245" s="2"/>
+      <c r="I245" s="2"/>
+      <c r="J245" s="2"/>
+      <c r="K245" s="2"/>
+      <c r="L245" s="2"/>
+      <c r="M245" s="6" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A232" s="7" t="s">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A246" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="M232" s="7" t="s">
+      <c r="M246" s="7" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A233" s="8" t="s">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A247" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="M233" s="7" t="s">
+      <c r="M247" s="7" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A234" s="7" t="s">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A248" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="M234" s="7" t="s">
+      <c r="M248" s="7" t="s">
         <v>392</v>
-      </c>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A236" t="s">
-        <v>393</v>
-      </c>
-      <c r="M236" s="7" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A237" t="s">
-        <v>395</v>
-      </c>
-      <c r="M237" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A238" t="s">
-        <v>396</v>
-      </c>
-      <c r="M238" s="7" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A239" t="s">
-        <v>397</v>
-      </c>
-      <c r="M239" s="7" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A241" t="s">
-        <v>413</v>
-      </c>
-      <c r="M241" s="7" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A242" t="s">
-        <v>414</v>
-      </c>
-      <c r="M242" s="7" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A243" t="s">
-        <v>416</v>
-      </c>
-      <c r="M243" s="7" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A244" t="s">
-        <v>418</v>
-      </c>
-      <c r="M244" s="7" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A246" t="s">
-        <v>422</v>
-      </c>
-      <c r="M246" s="7" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A247" t="s">
-        <v>421</v>
-      </c>
-      <c r="M247" s="7" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A248" t="s">
-        <v>426</v>
-      </c>
-      <c r="M248" s="7" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A249" t="s">
-        <v>428</v>
-      </c>
-      <c r="M249" s="7" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A250" t="s">
-        <v>429</v>
+        <v>393</v>
       </c>
       <c r="M250" s="7" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A251" t="s">
-        <v>432</v>
+        <v>395</v>
       </c>
       <c r="M251" s="7" t="s">
-        <v>431</v>
+        <v>399</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A252" t="s">
-        <v>433</v>
+        <v>396</v>
       </c>
       <c r="M252" s="7" t="s">
-        <v>434</v>
+        <v>398</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A253" t="s">
-        <v>435</v>
+        <v>397</v>
       </c>
       <c r="M253" s="7" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A254" t="s">
-        <v>437</v>
-      </c>
-      <c r="M254" s="7" t="s">
-        <v>438</v>
+        <v>400</v>
       </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A255" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="M255" s="7" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A256" t="s">
-        <v>441</v>
+        <v>414</v>
       </c>
       <c r="M256" s="7" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A257" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
       <c r="M257" s="7" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A258" t="s">
+        <v>418</v>
+      </c>
+      <c r="M258" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A260" t="s">
+        <v>422</v>
+      </c>
+      <c r="M260" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A261" t="s">
+        <v>421</v>
+      </c>
+      <c r="M261" s="7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A262" t="s">
+        <v>426</v>
+      </c>
+      <c r="M262" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A263" t="s">
+        <v>428</v>
+      </c>
+      <c r="M263" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A264" t="s">
+        <v>429</v>
+      </c>
+      <c r="M264" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A265" t="s">
+        <v>432</v>
+      </c>
+      <c r="M265" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A266" t="s">
+        <v>433</v>
+      </c>
+      <c r="M266" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A267" t="s">
+        <v>435</v>
+      </c>
+      <c r="M267" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A268" t="s">
+        <v>437</v>
+      </c>
+      <c r="M268" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A269" t="s">
+        <v>439</v>
+      </c>
+      <c r="M269" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A270" t="s">
+        <v>441</v>
+      </c>
+      <c r="M270" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A271" t="s">
+        <v>442</v>
+      </c>
+      <c r="M271" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A272" t="s">
         <v>445</v>
       </c>
-      <c r="M258" t="s">
+      <c r="M272" t="s">
         <v>444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat:new hats from seono
</commit_message>
<xml_diff>
--- a/HatTransData.xlsx
+++ b/HatTransData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeHat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A36F00F-52CF-4D89-82BB-E517850830B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84352001-B2D4-455E-819C-170834EC7813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="801">
   <si>
     <t>English</t>
   </si>
@@ -2345,6 +2345,129 @@
   </si>
   <si>
     <t>世界の王</t>
+  </si>
+  <si>
+    <t>Seono</t>
+  </si>
+  <si>
+    <t>セオノ作</t>
+  </si>
+  <si>
+    <t>SONDragon</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>ドラゴン</t>
+  </si>
+  <si>
+    <t>SONDragonColor</t>
+  </si>
+  <si>
+    <t>ドラゴンColor</t>
+  </si>
+  <si>
+    <t>SONFuwanekoCape</t>
+  </si>
+  <si>
+    <t>ふわねこケープ</t>
+  </si>
+  <si>
+    <t>SONFuwanekoCapeColor</t>
+  </si>
+  <si>
+    <t>ふわねこケープColor</t>
+  </si>
+  <si>
+    <t>SONGosurori</t>
+  </si>
+  <si>
+    <t>ゴスロリ</t>
+  </si>
+  <si>
+    <t>SONHeppokoAngle</t>
+  </si>
+  <si>
+    <t>へっぽこ天使</t>
+  </si>
+  <si>
+    <t>SONHighAngle</t>
+  </si>
+  <si>
+    <t>大天使</t>
+  </si>
+  <si>
+    <t>SONKitsune</t>
+  </si>
+  <si>
+    <t>Fox</t>
+  </si>
+  <si>
+    <t>狐</t>
+  </si>
+  <si>
+    <t>SONKyubi</t>
+  </si>
+  <si>
+    <t>九尾の狐</t>
+  </si>
+  <si>
+    <t>SONMaidMini</t>
+  </si>
+  <si>
+    <t>メイドミニ</t>
+  </si>
+  <si>
+    <t>SONManekiNeko</t>
+  </si>
+  <si>
+    <t>招き猫</t>
+  </si>
+  <si>
+    <t>SONRobeTypeA</t>
+  </si>
+  <si>
+    <t>ローブTypeA</t>
+  </si>
+  <si>
+    <t>SONRobeTypeB</t>
+  </si>
+  <si>
+    <t>ローブTypeB</t>
+  </si>
+  <si>
+    <t>SONShibainu</t>
+  </si>
+  <si>
+    <t>柴犬</t>
+  </si>
+  <si>
+    <t>SONVtuberStyle</t>
+  </si>
+  <si>
+    <t>VtuberStyle</t>
+  </si>
+  <si>
+    <t>SONWitch</t>
+  </si>
+  <si>
+    <t>Witch</t>
+  </si>
+  <si>
+    <t>SONWolf</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>狼</t>
+  </si>
+  <si>
+    <t>SONXmasCape</t>
+  </si>
+  <si>
+    <t>クリスマスケープ</t>
   </si>
 </sst>
 </file>
@@ -2420,7 +2543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2431,6 +2554,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2747,10 +2874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q421"/>
+  <dimension ref="A1:Q442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G259" sqref="G259"/>
+    <sheetView tabSelected="1" topLeftCell="A416" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B439" sqref="B439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -6579,6 +6706,186 @@
         <v>757</v>
       </c>
     </row>
+    <row r="424" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A424" t="s">
+        <v>760</v>
+      </c>
+      <c r="M424" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="425" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A425" t="s">
+        <v>762</v>
+      </c>
+      <c r="B425" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="M425" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="426" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A426" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="B426" s="7"/>
+      <c r="M426" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="427" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A427" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="B427" s="7"/>
+      <c r="M427" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="428" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A428" s="8" t="s">
+        <v>769</v>
+      </c>
+      <c r="B428" s="7"/>
+      <c r="M428" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="429" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A429" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="B429" s="7"/>
+      <c r="M429" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="430" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A430" t="s">
+        <v>773</v>
+      </c>
+      <c r="B430" s="7"/>
+      <c r="M430" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="431" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A431" t="s">
+        <v>775</v>
+      </c>
+      <c r="B431" s="7"/>
+      <c r="M431" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="432" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A432" t="s">
+        <v>777</v>
+      </c>
+      <c r="B432" t="s">
+        <v>778</v>
+      </c>
+      <c r="M432" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="433" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A433" t="s">
+        <v>780</v>
+      </c>
+      <c r="B433" s="7"/>
+      <c r="M433" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="434" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A434" t="s">
+        <v>782</v>
+      </c>
+      <c r="B434" s="7"/>
+      <c r="M434" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="435" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A435" t="s">
+        <v>784</v>
+      </c>
+      <c r="B435" s="7"/>
+      <c r="M435" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="436" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A436" t="s">
+        <v>786</v>
+      </c>
+      <c r="B436" s="7"/>
+      <c r="M436" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="437" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A437" t="s">
+        <v>788</v>
+      </c>
+      <c r="B437" s="7"/>
+      <c r="M437" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="438" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A438" t="s">
+        <v>790</v>
+      </c>
+      <c r="B438" s="7"/>
+      <c r="M438" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="439" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A439" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B439" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="M439" s="7" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="440" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A440" t="s">
+        <v>794</v>
+      </c>
+      <c r="B440" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="M440" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A441" t="s">
+        <v>796</v>
+      </c>
+      <c r="B441" t="s">
+        <v>797</v>
+      </c>
+      <c r="M441" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="442" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A442" t="s">
+        <v>799</v>
+      </c>
+      <c r="B442" s="7"/>
+      <c r="M442" t="s">
+        <v>800</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>